<commit_message>
maj liste de mots
</commit_message>
<xml_diff>
--- a/public/undercover_mots_francais.xlsx
+++ b/public/undercover_mots_francais.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10714"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thibaultbarral/Documents/Dev/Pro/undercover-game/public/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C44DB25E-39D6-6541-B541-6C80D4BB1D42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="115">
   <si>
     <t>Mot Commun</t>
   </si>
@@ -58,18 +64,12 @@
     <t>Maison</t>
   </si>
   <si>
-    <t>Stylo</t>
-  </si>
-  <si>
     <t>Pain</t>
   </si>
   <si>
     <t>Guitare</t>
   </si>
   <si>
-    <t>Ordinateur portable</t>
-  </si>
-  <si>
     <t>Avion</t>
   </si>
   <si>
@@ -79,9 +79,6 @@
     <t>Bouteille</t>
   </si>
   <si>
-    <t>Montagne</t>
-  </si>
-  <si>
     <t>Bureau</t>
   </si>
   <si>
@@ -109,7 +106,94 @@
     <t>Lit</t>
   </si>
   <si>
-    <t>Souris</t>
+    <t>Pâtes</t>
+  </si>
+  <si>
+    <t>Hamburger</t>
+  </si>
+  <si>
+    <t>Crêpe</t>
+  </si>
+  <si>
+    <t>Chocolat</t>
+  </si>
+  <si>
+    <t>Bière</t>
+  </si>
+  <si>
+    <t>Lait</t>
+  </si>
+  <si>
+    <t>Salade</t>
+  </si>
+  <si>
+    <t>Télévision</t>
+  </si>
+  <si>
+    <t>Ordinateur</t>
+  </si>
+  <si>
+    <t>Couteau</t>
+  </si>
+  <si>
+    <t>Verre</t>
+  </si>
+  <si>
+    <t>Sac</t>
+  </si>
+  <si>
+    <t>Montre</t>
+  </si>
+  <si>
+    <t>Clé</t>
+  </si>
+  <si>
+    <t>Chat</t>
+  </si>
+  <si>
+    <t>Vache</t>
+  </si>
+  <si>
+    <t>Cheval</t>
+  </si>
+  <si>
+    <t>Poule</t>
+  </si>
+  <si>
+    <t>Poisson</t>
+  </si>
+  <si>
+    <t>Oiseau</t>
+  </si>
+  <si>
+    <t>Singe</t>
+  </si>
+  <si>
+    <t>Cochon</t>
+  </si>
+  <si>
+    <t>Serpent</t>
+  </si>
+  <si>
+    <t>Drone</t>
+  </si>
+  <si>
+    <t>Voiture électrique</t>
+  </si>
+  <si>
+    <t>Smartphone</t>
+  </si>
+  <si>
+    <t>Console</t>
+  </si>
+  <si>
+    <t>Micro</t>
+  </si>
+  <si>
+    <t>Disque dur</t>
+  </si>
+  <si>
+    <t>Réfrigérateur</t>
   </si>
   <si>
     <t>Banane</t>
@@ -148,30 +232,18 @@
     <t>Appartement</t>
   </si>
   <si>
-    <t>Crayon</t>
-  </si>
-  <si>
     <t>Gâteau</t>
   </si>
   <si>
     <t>Violon</t>
   </si>
   <si>
-    <t>Ordinateur de bureau</t>
-  </si>
-  <si>
     <t>Hélicoptère</t>
   </si>
   <si>
-    <t>Montre</t>
-  </si>
-  <si>
     <t>Tasse</t>
   </si>
   <si>
-    <t>Colline</t>
-  </si>
-  <si>
     <t>Table</t>
   </si>
   <si>
@@ -199,14 +271,107 @@
     <t>Canapé</t>
   </si>
   <si>
-    <t>Rat</t>
+    <t>Couscous</t>
+  </si>
+  <si>
+    <t>Tacos</t>
+  </si>
+  <si>
+    <t>Muffin</t>
+  </si>
+  <si>
+    <t>Caramel</t>
+  </si>
+  <si>
+    <t>Whisky</t>
+  </si>
+  <si>
+    <t>Taboulé</t>
+  </si>
+  <si>
+    <t>Pastèque</t>
+  </si>
+  <si>
+    <t>Projecteur</t>
+  </si>
+  <si>
+    <t>Imprimante</t>
+  </si>
+  <si>
+    <t>Torche</t>
+  </si>
+  <si>
+    <t>Ciseaux</t>
+  </si>
+  <si>
+    <t>Sac à dos</t>
+  </si>
+  <si>
+    <t>Pantoufles</t>
+  </si>
+  <si>
+    <t>Cadenas</t>
+  </si>
+  <si>
+    <t>Télécommande</t>
+  </si>
+  <si>
+    <t>Renard</t>
+  </si>
+  <si>
+    <t>Panthère</t>
+  </si>
+  <si>
+    <t>Rhinocéros</t>
+  </si>
+  <si>
+    <t>Chameau</t>
+  </si>
+  <si>
+    <t>Autruche</t>
+  </si>
+  <si>
+    <t>Méduse</t>
+  </si>
+  <si>
+    <t>Hibou</t>
+  </si>
+  <si>
+    <t>Kangourou</t>
+  </si>
+  <si>
+    <t>Lapin</t>
+  </si>
+  <si>
+    <t>Scorpion</t>
+  </si>
+  <si>
+    <t>Satellite</t>
+  </si>
+  <si>
+    <t>Scooter</t>
+  </si>
+  <si>
+    <t>Smartwatch</t>
+  </si>
+  <si>
+    <t>Arcade</t>
+  </si>
+  <si>
+    <t>Caméra</t>
+  </si>
+  <si>
+    <t>Cloud</t>
+  </si>
+  <si>
+    <t>Micro-ondes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -269,13 +434,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -313,7 +486,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -347,6 +520,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -381,9 +555,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -556,14 +731,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="150" workbookViewId="0">
+      <selection activeCell="A60" sqref="A60:XFD60"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.83203125" customWidth="1"/>
+    <col min="2" max="2" width="22.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -571,244 +752,492 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>28</v>
       </c>
       <c r="B28" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>29</v>
       </c>
       <c r="B29" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>30</v>
       </c>
       <c r="B30" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>31</v>
       </c>
       <c r="B31" t="s">
-        <v>61</v>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>32</v>
+      </c>
+      <c r="B32" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>33</v>
+      </c>
+      <c r="B33" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>34</v>
+      </c>
+      <c r="B34" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>2</v>
+      </c>
+      <c r="B35" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>21</v>
+      </c>
+      <c r="B38" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>37</v>
+      </c>
+      <c r="B39" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>38</v>
+      </c>
+      <c r="B40" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>39</v>
+      </c>
+      <c r="B41" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>26</v>
+      </c>
+      <c r="B42" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>40</v>
+      </c>
+      <c r="B43" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>41</v>
+      </c>
+      <c r="B44" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>7</v>
+      </c>
+      <c r="B45" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>3</v>
+      </c>
+      <c r="B46" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>42</v>
+      </c>
+      <c r="B47" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>43</v>
+      </c>
+      <c r="B48" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>44</v>
+      </c>
+      <c r="B49" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>45</v>
+      </c>
+      <c r="B50" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>46</v>
+      </c>
+      <c r="B51" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>47</v>
+      </c>
+      <c r="B52" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>48</v>
+      </c>
+      <c r="B53" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>49</v>
+      </c>
+      <c r="B54" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>50</v>
+      </c>
+      <c r="B55" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>51</v>
+      </c>
+      <c r="B56" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>52</v>
+      </c>
+      <c r="B57" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>53</v>
+      </c>
+      <c r="B58" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>54</v>
+      </c>
+      <c r="B59" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>55</v>
+      </c>
+      <c r="B60" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>56</v>
+      </c>
+      <c r="B61" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>57</v>
+      </c>
+      <c r="B62" t="s">
+        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>